<commit_message>
import export data mahasiswa
</commit_message>
<xml_diff>
--- a/_uploads/format_excel/FormatMahasiswa.xlsx
+++ b/_uploads/format_excel/FormatMahasiswa.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>No</t>
   </si>
@@ -93,13 +93,85 @@
   </si>
   <si>
     <t>17121057@student.mercubuana-yogya.ac.id</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>Keterangan :</t>
+  </si>
+  <si>
+    <t>Jurusan</t>
+  </si>
+  <si>
+    <t>Sistem Informasi</t>
+  </si>
+  <si>
+    <t>Informatika</t>
+  </si>
+  <si>
+    <t>Manajemen</t>
+  </si>
+  <si>
+    <t>Akuntansi</t>
+  </si>
+  <si>
+    <t>Agroteknologi</t>
+  </si>
+  <si>
+    <t>Industri Peternakan</t>
+  </si>
+  <si>
+    <t>Teknologi Pangan</t>
+  </si>
+  <si>
+    <t>Ilmu Pangan</t>
+  </si>
+  <si>
+    <t>Psikologi</t>
+  </si>
+  <si>
+    <t>Pendidikan Bahasa Inggris</t>
+  </si>
+  <si>
+    <t>Pendidikan Matematika</t>
+  </si>
+  <si>
+    <t>Bimbingan Konseling</t>
+  </si>
+  <si>
+    <t>Ilmu Keolahragaan</t>
+  </si>
+  <si>
+    <t>Ilmu Komunikasi</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Kaprodi</t>
+  </si>
+  <si>
+    <t>Dosen</t>
+  </si>
+  <si>
+    <t>Tata Usaha</t>
+  </si>
+  <si>
+    <t>Mahasiswa</t>
+  </si>
+  <si>
+    <t>Administrasi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,16 +193,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -138,15 +230,203 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -428,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,9 +723,14 @@
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,10 +752,13 @@
       <c r="G1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>17121050</v>
@@ -490,10 +778,13 @@
       <c r="G2">
         <v>2017</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>17121051</v>
@@ -513,10 +804,17 @@
       <c r="G3">
         <v>2017</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>17121052</v>
@@ -536,10 +834,19 @@
       <c r="G4">
         <v>2017</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>17121053</v>
@@ -559,10 +866,31 @@
       <c r="G5">
         <v>2017</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>17121054</v>
@@ -582,10 +910,31 @@
       <c r="G6">
         <v>2017</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="J6" s="11">
+        <v>1</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="13">
+        <v>1</v>
+      </c>
+      <c r="N6" s="11">
+        <v>1</v>
+      </c>
+      <c r="O6" s="12">
+        <v>1</v>
+      </c>
+      <c r="P6" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>17121055</v>
@@ -605,10 +954,31 @@
       <c r="G7">
         <v>2017</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="J7" s="4">
+        <v>2</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="6">
+        <v>2</v>
+      </c>
+      <c r="N7" s="4">
+        <v>2</v>
+      </c>
+      <c r="O7" s="5">
+        <v>2</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>17121056</v>
@@ -628,10 +998,31 @@
       <c r="G8">
         <v>2017</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="J8" s="4">
+        <v>3</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="6">
+        <v>3</v>
+      </c>
+      <c r="N8" s="4">
+        <v>3</v>
+      </c>
+      <c r="O8" s="5">
+        <v>3</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>17121057</v>
@@ -650,6 +1041,146 @@
       </c>
       <c r="G9">
         <v>2017</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="J9" s="4">
+        <v>4</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="6">
+        <v>4</v>
+      </c>
+      <c r="N9" s="4">
+        <v>4</v>
+      </c>
+      <c r="O9" s="5">
+        <v>4</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J10" s="4">
+        <v>5</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" s="6">
+        <v>5</v>
+      </c>
+      <c r="N10" s="8">
+        <v>5</v>
+      </c>
+      <c r="O10" s="9">
+        <v>5</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J11" s="4">
+        <v>6</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J12" s="4">
+        <v>7</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J13" s="4">
+        <v>8</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J14" s="4">
+        <v>9</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J15" s="4">
+        <v>10</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J16" s="4">
+        <v>11</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L16" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J17" s="4">
+        <v>12</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L17" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J18" s="4">
+        <v>13</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="10:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J19" s="8">
+        <v>14</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" s="10">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
insert and update data student & lecturer in TU
</commit_message>
<xml_diff>
--- a/_uploads/format_excel/FormatMahasiswa.xlsx
+++ b/_uploads/format_excel/FormatMahasiswa.xlsx
@@ -68,9 +68,6 @@
     <t>Bagas Abimanyu</t>
   </si>
   <si>
-    <t>class</t>
-  </si>
-  <si>
     <t>17121050@student.mercubuana-yogya.ac.id</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>Administrasi</t>
+  </si>
+  <si>
+    <t>angatan</t>
   </si>
 </sst>
 </file>
@@ -711,7 +711,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,10 +750,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>17121050</v>
@@ -793,7 +793,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>17121051</v>
@@ -808,7 +808,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K3" s="3"/>
     </row>
@@ -823,7 +823,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>17121052</v>
@@ -838,10 +838,10 @@
         <v>4</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -855,7 +855,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>17121053</v>
@@ -873,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L5" s="16" t="s">
         <v>5</v>
@@ -882,10 +882,10 @@
         <v>0</v>
       </c>
       <c r="O5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5" s="16" t="s">
         <v>40</v>
-      </c>
-      <c r="P5" s="16" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -899,7 +899,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>17121054</v>
@@ -917,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L6" s="13">
         <v>1</v>
@@ -929,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="P6" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -943,7 +943,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7">
         <v>17121055</v>
@@ -961,7 +961,7 @@
         <v>2</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L7" s="6">
         <v>2</v>
@@ -973,7 +973,7 @@
         <v>2</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -987,7 +987,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8">
         <v>17121056</v>
@@ -1005,7 +1005,7 @@
         <v>3</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L8" s="6">
         <v>3</v>
@@ -1017,7 +1017,7 @@
         <v>3</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1031,7 +1031,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>17121057</v>
@@ -1049,7 +1049,7 @@
         <v>4</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L9" s="6">
         <v>4</v>
@@ -1061,7 +1061,7 @@
         <v>4</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1069,7 +1069,7 @@
         <v>5</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L10" s="6">
         <v>5</v>
@@ -1081,7 +1081,7 @@
         <v>5</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1089,7 +1089,7 @@
         <v>6</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L11" s="6">
         <v>6</v>
@@ -1100,7 +1100,7 @@
         <v>7</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L12" s="6">
         <v>7</v>
@@ -1111,7 +1111,7 @@
         <v>8</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L13" s="6">
         <v>8</v>
@@ -1122,7 +1122,7 @@
         <v>9</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L14" s="6">
         <v>9</v>
@@ -1133,7 +1133,7 @@
         <v>10</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L15" s="6">
         <v>10</v>
@@ -1144,7 +1144,7 @@
         <v>11</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L16" s="6">
         <v>11</v>
@@ -1155,7 +1155,7 @@
         <v>12</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L17" s="6">
         <v>12</v>
@@ -1166,7 +1166,7 @@
         <v>13</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L18" s="6">
         <v>13</v>
@@ -1177,7 +1177,7 @@
         <v>14</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L19" s="10">
         <v>14</v>

</xml_diff>